<commit_message>
Modified files on B2
</commit_message>
<xml_diff>
--- a/seamonitor/backend/data/temperature.xlsx
+++ b/seamonitor/backend/data/temperature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\软件工程\Lab5项目管理\git提交\seamonitor\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3869551-63EA-4099-B7CA-4E7CEC5DC152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427912A2-5B51-4B7A-B3EE-70E9F109810A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -379,6 +379,11 @@
         <v>60</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.65">
+      <c r="A4">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified four files on C4
</commit_message>
<xml_diff>
--- a/seamonitor/backend/data/temperature.xlsx
+++ b/seamonitor/backend/data/temperature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\软件工程\Lab5项目管理\git提交\seamonitor\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427912A2-5B51-4B7A-B3EE-70E9F109810A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2698D7AB-C7E7-4C06-A904-1D61EC5F8E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -379,11 +379,6 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A4">
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified four files on B3
</commit_message>
<xml_diff>
--- a/seamonitor/backend/data/temperature.xlsx
+++ b/seamonitor/backend/data/temperature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\软件工程\Lab5项目管理\git提交\seamonitor\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3869551-63EA-4099-B7CA-4E7CEC5DC152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6D9BDE-9CC7-4D7A-9091-E500DE59693A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -379,6 +379,11 @@
         <v>60</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.65">
+      <c r="A4">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>